<commit_message>
Updated report: finished except for convergence diagrams
</commit_message>
<xml_diff>
--- a/ContinuationReport_GANNT.xlsx
+++ b/ContinuationReport_GANNT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="72" windowWidth="20100" windowHeight="7944"/>
+    <workbookView xWindow="288" yWindow="72" windowWidth="20100" windowHeight="7944" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>Task</t>
   </si>
@@ -145,13 +145,37 @@
   </si>
   <si>
     <t>Thesis chapter 4 (review of convergence methods, paper 4)</t>
+  </si>
+  <si>
+    <t>Convergence analysis</t>
+  </si>
+  <si>
+    <t>Submit disparity paper</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Discussion</t>
+  </si>
+  <si>
+    <t>Complete thesis draft</t>
+  </si>
+  <si>
+    <t>Write up convergence methods and results</t>
+  </si>
+  <si>
+    <t>Finish disparity paper: introduction and discussion</t>
+  </si>
+  <si>
+    <t>Morphometric error checking</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,8 +197,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,8 +254,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -464,11 +501,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -494,16 +542,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -519,15 +557,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -541,6 +570,44 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,10 +914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:M37"/>
+  <dimension ref="A3:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView topLeftCell="C1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -860,64 +927,64 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="40"/>
-      <c r="C3" s="36">
+      <c r="B3" s="33"/>
+      <c r="C3" s="43">
         <v>2014</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="38">
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="46">
         <v>2015</v>
       </c>
-      <c r="K3" s="39"/>
+      <c r="K3" s="47"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="35" t="s">
+      <c r="J4" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="31" t="s">
+      <c r="K4" s="27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="2"/>
-      <c r="J5" s="49"/>
+      <c r="J5" s="42"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="28" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="15"/>
@@ -926,7 +993,7 @@
       <c r="K6" s="13"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="28" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="16"/>
@@ -935,7 +1002,7 @@
       <c r="K7" s="13"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="28" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="17"/>
@@ -944,7 +1011,7 @@
       <c r="K8" s="13"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="28" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="17"/>
@@ -955,7 +1022,7 @@
       <c r="K9" s="13"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="28" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="17"/>
@@ -965,7 +1032,7 @@
       <c r="K10" s="13"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="17"/>
@@ -976,7 +1043,7 @@
       <c r="K11" s="13"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="17"/>
@@ -984,34 +1051,34 @@
       <c r="I12" s="3"/>
       <c r="J12" s="9"/>
       <c r="K12" s="13"/>
-      <c r="M12" s="31" t="s">
+      <c r="M12" s="27" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="17"/>
       <c r="J13" s="10"/>
       <c r="K13" s="13"/>
-      <c r="M13" s="41" t="s">
+      <c r="M13" s="34" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="17"/>
       <c r="J14" s="11"/>
       <c r="K14" s="19"/>
-      <c r="M14" s="42" t="s">
+      <c r="M14" s="35" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="29" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="21"/>
@@ -1023,63 +1090,63 @@
       <c r="I15" s="8"/>
       <c r="J15" s="22"/>
       <c r="K15" s="23"/>
-      <c r="M15" s="43" t="s">
+      <c r="M15" s="36" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="27">
+      <c r="C16" s="48">
         <v>2015</v>
       </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="26"/>
-      <c r="M16" s="44" t="s">
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="50"/>
+      <c r="M16" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="31" t="s">
+      <c r="H17" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="I17" s="31" t="s">
+      <c r="I17" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="J17" s="31" t="s">
+      <c r="J17" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="K17" s="31" t="s">
+      <c r="K17" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="M17" s="45" t="s">
+      <c r="M17" s="38" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="26" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="15"/>
@@ -1091,23 +1158,23 @@
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
       <c r="K18" s="18"/>
-      <c r="M18" s="46" t="s">
+      <c r="M18" s="39" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="26" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="4"/>
       <c r="K19" s="13"/>
-      <c r="M19" s="47" t="s">
+      <c r="M19" s="40" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="26" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="17"/>
@@ -1116,7 +1183,7 @@
       <c r="K20" s="13"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="26" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="17"/>
@@ -1125,7 +1192,7 @@
       <c r="K21" s="13"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="17"/>
@@ -1133,7 +1200,7 @@
       <c r="K22" s="13"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="26" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="17"/>
@@ -1142,7 +1209,7 @@
       <c r="K23" s="13"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="26" t="s">
         <v>39</v>
       </c>
       <c r="C24" s="17"/>
@@ -1151,7 +1218,7 @@
       <c r="K24" s="13"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="26" t="s">
         <v>41</v>
       </c>
       <c r="C25" s="17"/>
@@ -1160,7 +1227,7 @@
       <c r="K25" s="13"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="26" t="s">
         <v>42</v>
       </c>
       <c r="C26" s="17"/>
@@ -1169,7 +1236,7 @@
       <c r="K26" s="13"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="26" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="17"/>
@@ -1188,25 +1255,87 @@
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
-      <c r="K28" s="48"/>
+      <c r="K28" s="41"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D37" s="2"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="56"/>
+      <c r="K32" s="56"/>
+      <c r="L32" s="56"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H33" s="57"/>
+      <c r="I33" s="57"/>
+      <c r="J33" s="57"/>
+      <c r="K33" s="57"/>
+      <c r="L33" s="55"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H34" s="57"/>
+      <c r="I34" s="57"/>
+      <c r="J34" s="57"/>
+      <c r="K34" s="57"/>
+      <c r="L34" s="55"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H35" s="57"/>
+      <c r="I35" s="57"/>
+      <c r="J35" s="57"/>
+      <c r="K35" s="57"/>
+      <c r="L35" s="55"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H36" s="57"/>
+      <c r="I36" s="57"/>
+      <c r="J36" s="57"/>
+      <c r="K36" s="57"/>
+      <c r="L36" s="55"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H37" s="57"/>
+      <c r="I37" s="57"/>
+      <c r="J37" s="57"/>
+      <c r="K37" s="57"/>
+      <c r="L37" s="55"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="57"/>
+      <c r="K38" s="57"/>
+      <c r="L38" s="55"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H39" s="57"/>
+      <c r="I39" s="57"/>
+      <c r="J39" s="57"/>
+      <c r="K39" s="57"/>
+      <c r="L39" s="55"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H40" s="57"/>
+      <c r="I40" s="57"/>
+      <c r="J40" s="57"/>
+      <c r="K40" s="57"/>
+      <c r="L40" s="55"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="55"/>
+      <c r="B41" s="55"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="57"/>
+      <c r="J41" s="57"/>
+      <c r="K41" s="57"/>
+      <c r="L41" s="58"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C42" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1221,12 +1350,145 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="E12:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="5" max="5" width="43" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="12" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E12" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E13" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="62"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="61"/>
+      <c r="L13" s="27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E14" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="52"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="13"/>
+      <c r="L14" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E15" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="59"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="13"/>
+      <c r="L15" s="35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E16" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="59"/>
+      <c r="H16" s="58"/>
+      <c r="J16" s="13"/>
+      <c r="L16" s="36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E17" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="52"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="13"/>
+      <c r="L17" s="39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E18" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="52"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="13"/>
+      <c r="L18" s="40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E19" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="52"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E20" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="52"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="13"/>
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E21" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="53"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="41"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Final versions of the report and table of contents ready to submit to the committee. I re-named the report file and added a table of completion dates instead of the GANTT chart
</commit_message>
<xml_diff>
--- a/ContinuationReport_GANNT.xlsx
+++ b/ContinuationReport_GANNT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
   <si>
     <t>Task</t>
   </si>
@@ -150,25 +150,76 @@
     <t>Convergence analysis</t>
   </si>
   <si>
-    <t>Submit disparity paper</t>
-  </si>
-  <si>
     <t>Introduction</t>
   </si>
   <si>
     <t>Discussion</t>
   </si>
   <si>
-    <t>Complete thesis draft</t>
-  </si>
-  <si>
-    <t>Write up convergence methods and results</t>
-  </si>
-  <si>
-    <t>Finish disparity paper: introduction and discussion</t>
-  </si>
-  <si>
-    <t>Morphometric error checking</t>
+    <t>Convergence write up</t>
+  </si>
+  <si>
+    <t>Error checking analysis</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Number of weeks</t>
+  </si>
+  <si>
+    <t>Finish disparity chapter</t>
+  </si>
+  <si>
+    <t>1st September</t>
+  </si>
+  <si>
+    <t>12th September</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15th September </t>
+  </si>
+  <si>
+    <t>26th September</t>
+  </si>
+  <si>
+    <t>Data collection chapter write up</t>
+  </si>
+  <si>
+    <t>29th September</t>
+  </si>
+  <si>
+    <t>3rd October</t>
+  </si>
+  <si>
+    <t>6th October</t>
+  </si>
+  <si>
+    <t>24th October</t>
+  </si>
+  <si>
+    <t>27th October</t>
+  </si>
+  <si>
+    <t>31st October</t>
+  </si>
+  <si>
+    <t>3rd November</t>
+  </si>
+  <si>
+    <t>21st November</t>
+  </si>
+  <si>
+    <t>24th November</t>
+  </si>
+  <si>
+    <t>12th December</t>
+  </si>
+  <si>
+    <t>30th January</t>
   </si>
 </sst>
 </file>
@@ -205,7 +256,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,14 +305,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -501,22 +546,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -557,9 +591,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
@@ -570,6 +601,14 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -592,22 +631,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,20 +956,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="33"/>
-      <c r="C3" s="43">
+      <c r="B3" s="32"/>
+      <c r="C3" s="48">
         <v>2014</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="46">
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="51">
         <v>2015</v>
       </c>
-      <c r="K3" s="47"/>
+      <c r="K3" s="52"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="27" t="s">
@@ -980,7 +1009,7 @@
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="2"/>
-      <c r="J5" s="42"/>
+      <c r="J5" s="41"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
@@ -1062,7 +1091,7 @@
       <c r="C13" s="17"/>
       <c r="J13" s="10"/>
       <c r="K13" s="13"/>
-      <c r="M13" s="34" t="s">
+      <c r="M13" s="33" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1073,7 +1102,7 @@
       <c r="C14" s="17"/>
       <c r="J14" s="11"/>
       <c r="K14" s="19"/>
-      <c r="M14" s="35" t="s">
+      <c r="M14" s="34" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1090,23 +1119,23 @@
       <c r="I15" s="8"/>
       <c r="J15" s="22"/>
       <c r="K15" s="23"/>
-      <c r="M15" s="36" t="s">
+      <c r="M15" s="35" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="48">
+      <c r="C16" s="53">
         <v>2015</v>
       </c>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="50"/>
-      <c r="M16" s="37" t="s">
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="55"/>
+      <c r="M16" s="36" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1141,7 +1170,7 @@
       <c r="K17" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="M17" s="38" t="s">
+      <c r="M17" s="37" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1158,7 +1187,7 @@
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
       <c r="K18" s="18"/>
-      <c r="M18" s="39" t="s">
+      <c r="M18" s="38" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1169,7 +1198,7 @@
       <c r="C19" s="17"/>
       <c r="D19" s="4"/>
       <c r="K19" s="13"/>
-      <c r="M19" s="40" t="s">
+      <c r="M19" s="39" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1255,87 +1284,87 @@
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
-      <c r="K28" s="41"/>
+      <c r="K28" s="40"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="56"/>
-      <c r="K32" s="56"/>
-      <c r="L32" s="56"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="45"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H33" s="57"/>
-      <c r="I33" s="57"/>
-      <c r="J33" s="57"/>
-      <c r="K33" s="57"/>
-      <c r="L33" s="55"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="44"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H34" s="57"/>
-      <c r="I34" s="57"/>
-      <c r="J34" s="57"/>
-      <c r="K34" s="57"/>
-      <c r="L34" s="55"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="46"/>
+      <c r="K34" s="46"/>
+      <c r="L34" s="44"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H35" s="57"/>
-      <c r="I35" s="57"/>
-      <c r="J35" s="57"/>
-      <c r="K35" s="57"/>
-      <c r="L35" s="55"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="46"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="44"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H36" s="57"/>
-      <c r="I36" s="57"/>
-      <c r="J36" s="57"/>
-      <c r="K36" s="57"/>
-      <c r="L36" s="55"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="46"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="44"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H37" s="57"/>
-      <c r="I37" s="57"/>
-      <c r="J37" s="57"/>
-      <c r="K37" s="57"/>
-      <c r="L37" s="55"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="46"/>
+      <c r="L37" s="44"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H38" s="57"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="57"/>
-      <c r="K38" s="57"/>
-      <c r="L38" s="55"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="44"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H39" s="57"/>
-      <c r="I39" s="57"/>
-      <c r="J39" s="57"/>
-      <c r="K39" s="57"/>
-      <c r="L39" s="55"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="44"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H40" s="57"/>
-      <c r="I40" s="57"/>
-      <c r="J40" s="57"/>
-      <c r="K40" s="57"/>
-      <c r="L40" s="55"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="44"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41" s="55"/>
-      <c r="B41" s="55"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="57"/>
-      <c r="E41" s="57"/>
-      <c r="F41" s="57"/>
-      <c r="G41" s="58"/>
-      <c r="H41" s="57"/>
-      <c r="I41" s="57"/>
-      <c r="J41" s="57"/>
-      <c r="K41" s="57"/>
-      <c r="L41" s="58"/>
+      <c r="A41" s="44"/>
+      <c r="B41" s="44"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="46"/>
+      <c r="I41" s="46"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="46"/>
+      <c r="L41" s="47"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C42" s="57"/>
+      <c r="C42" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1350,146 +1379,152 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E12:L21"/>
+  <dimension ref="E12:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="6" customWidth="1"/>
     <col min="5" max="5" width="43" customWidth="1"/>
-    <col min="12" max="12" width="14.77734375" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="12" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E12" s="27" t="s">
         <v>0</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="H12" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="J12" s="32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="5:12" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E13" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="62"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="61"/>
-      <c r="L13" s="27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="5:12" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F13" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E14" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E15" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E16" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E17" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E18" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="52"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="58"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="13"/>
-      <c r="L14" s="34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E15" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="59"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="13"/>
-      <c r="L15" s="35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E16" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="59"/>
-      <c r="H16" s="58"/>
-      <c r="J16" s="13"/>
-      <c r="L16" s="36" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E17" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="52"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="13"/>
-      <c r="L17" s="39" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E18" s="28" t="s">
+      <c r="F18" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E19" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="52"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="63"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="13"/>
-      <c r="L18" s="40" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E19" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="52"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="63"/>
-      <c r="I19" s="63"/>
-      <c r="J19" s="13"/>
-    </row>
-    <row r="20" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E20" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="52"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="64"/>
-      <c r="J20" s="13"/>
-    </row>
-    <row r="21" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="F19" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E20" s="28"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="60"/>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E21" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="53"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="41"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" s="61"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>